<commit_message>
Login user Test Suit has been finished
</commit_message>
<xml_diff>
--- a/Data Test Plan.xlsx
+++ b/Data Test Plan.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramingProjects\KatalonProjects\AcademiaQA_Katalon_YourStoreSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D9BAB0-2CED-4E2B-8EFE-84CD5F477660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD468E0-4DE4-49E9-9204-7ADBD9B5DEE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15150" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="register new user" sheetId="1" r:id="rId1"/>
-    <sheet name="register exist user" sheetId="5" r:id="rId2"/>
-    <sheet name="register user without param" sheetId="4" r:id="rId3"/>
-    <sheet name="register user without politics" sheetId="6" r:id="rId4"/>
+    <sheet name="login user with correct values" sheetId="9" r:id="rId1"/>
+    <sheet name="login user with error values" sheetId="8" r:id="rId2"/>
+    <sheet name="login user without params" sheetId="7" r:id="rId3"/>
+    <sheet name="register new user" sheetId="1" r:id="rId4"/>
+    <sheet name="register exist user" sheetId="5" r:id="rId5"/>
+    <sheet name="register user without param" sheetId="4" r:id="rId6"/>
+    <sheet name="register user without politics" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
   <si>
     <t>first_name</t>
   </si>
@@ -91,13 +94,34 @@
   </si>
   <si>
     <t>correo1231234@gmail1.com</t>
+  </si>
+  <si>
+    <t>expected text</t>
+  </si>
+  <si>
+    <t>email12343565gmail.com</t>
+  </si>
+  <si>
+    <t>No match for E-Mail Address and/or Password.</t>
+  </si>
+  <si>
+    <t>email12343565@gmail.com</t>
+  </si>
+  <si>
+    <t>correo1231231@gmail.com</t>
+  </si>
+  <si>
+    <t>claveIncorrecta</t>
+  </si>
+  <si>
+    <t>email122321@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +133,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,6 +448,194 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D688D313-A153-4B07-BE99-78DF74E9F2FA}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{9C246780-B7B7-4061-9EFF-CDDF94DA342D}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1C987923-42D9-4A8F-86CA-0F0D7AA43B3D}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{D920B9BA-768D-4C82-A0C2-F5C66B5AB7BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F1001E-6F7F-4C7C-A2FD-02B666C1D2CD}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5D243A30-BBF8-44D3-8A05-D3DFA6E800E9}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{C10EDF9D-42A8-494C-B5D6-2C70175A9098}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{6925AE67-A9B5-48E8-BC9F-03082B6909BF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5001D4CB-50DF-4503-B4A8-E3DD99DCFDA6}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00F26968-B983-4F77-9E33-3931D6346F7F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -483,12 +701,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C99F7E-6ADD-4D44-A855-C1C4567B9B47}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C1" sqref="C1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +762,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FF3E77-2386-4A20-A311-812D5CA21552}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -676,12 +894,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3909D674-8546-4FD6-8D95-6410B3166705}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding test cases for basic shopping cart
</commit_message>
<xml_diff>
--- a/Data Test Plan.xlsx
+++ b/Data Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramingProjects\KatalonProjects\AcademiaQA_Katalon_YourStoreSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD468E0-4DE4-49E9-9204-7ADBD9B5DEE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AE6FB3-DC3C-4D99-862B-271AB4157724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login user with correct values" sheetId="9" r:id="rId1"/>
@@ -21,17 +21,23 @@
     <sheet name="register user without param" sheetId="4" r:id="rId6"/>
     <sheet name="register user without politics" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="28">
   <si>
     <t>first_name</t>
   </si>
@@ -114,7 +120,7 @@
     <t>claveIncorrecta</t>
   </si>
   <si>
-    <t>email122321@gmail.com</t>
+    <t>email123123@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D688D313-A153-4B07-BE99-78DF74E9F2FA}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,25 +485,16 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{9C246780-B7B7-4061-9EFF-CDDF94DA342D}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{1C987923-42D9-4A8F-86CA-0F0D7AA43B3D}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{D920B9BA-768D-4C82-A0C2-F5C66B5AB7BD}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{FA290A84-B868-45CC-91AC-67EDED84ECD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -898,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3909D674-8546-4FD6-8D95-6410B3166705}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>

</xml_diff>